<commit_message>
Make legend the correct name for descriptors and detectors
</commit_message>
<xml_diff>
--- a/Different Detector and Descriptor.xlsx
+++ b/Different Detector and Descriptor.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
   <si>
     <t>SHITOMASI/BRISK</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>BRISK/ORB</t>
-  </si>
-  <si>
-    <t>Lidar TTC</t>
   </si>
 </sst>
 </file>
@@ -111,10 +108,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+  <cellXfs count="1">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -383,12 +377,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>542293</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>243478</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8220075" cy="3429000"/>
+    <xdr:ext cx="10001250" cy="3838575"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1" name="Chart 0"/>
@@ -414,7 +408,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="B1" sqref="B1:M19"/>
@@ -426,25 +420,25 @@
     <col min="2" max="2" style="0" width="13.570612980769232" customWidth="1"/>
     <col min="3" max="4" style="0" width="12.99921875" customWidth="1"/>
     <col min="5" max="5" style="0" width="12.142127403846155" customWidth="1"/>
-    <col min="6" max="256" style="0" width="9.142307692307693"/>
+    <col min="6" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="inlineStr">
         <is>
           <t>Frame</t>
         </is>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -471,15 +465,17 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Lidar TTC</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>22.02</v>
       </c>
       <c r="C2">
@@ -515,15 +511,15 @@
       <c r="M2">
         <v>40.810000000000002</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2">
         <v>12.51</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>14.99</v>
       </c>
       <c r="C3">
@@ -559,15 +555,15 @@
       <c r="M3">
         <v>15.859999999999999</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3">
         <v>12.609999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>6.1699999999999999</v>
       </c>
       <c r="C4">
@@ -603,15 +599,15 @@
       <c r="M4">
         <v>11.42</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4">
         <v>14.09</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>10.41</v>
       </c>
       <c r="C5">
@@ -647,15 +643,15 @@
       <c r="M5">
         <v>21.149999999999999</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5">
         <v>16.690000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>22.640000000000001</v>
       </c>
       <c r="C6">
@@ -691,15 +687,15 @@
       <c r="M6">
         <v>49.039999999999999</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6">
         <v>15.91</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>18.699999999999999</v>
       </c>
       <c r="C7">
@@ -735,15 +731,15 @@
       <c r="M7">
         <v>12.24</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7">
         <v>12.67</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>9.4700000000000006</v>
       </c>
       <c r="C8">
@@ -779,15 +775,15 @@
       <c r="M8">
         <v>21.539999999999999</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8">
         <v>11.98</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>18.170000000000002</v>
       </c>
       <c r="C9">
@@ -823,15 +819,15 @@
       <c r="M9">
         <v>18.760000000000002</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9">
         <v>13.119999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>13.25</v>
       </c>
       <c r="C10">
@@ -867,15 +863,15 @@
       <c r="M10">
         <v>13.210000000000001</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10">
         <v>13.02</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>23.899999999999999</v>
       </c>
       <c r="C11">
@@ -911,15 +907,15 @@
       <c r="M11">
         <v>15.960000000000001</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11">
         <v>11.17</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>7.4699999999999998</v>
       </c>
       <c r="C12">
@@ -955,15 +951,15 @@
       <c r="M12">
         <v>9.7300000000000004</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12">
         <v>12.81</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>7.8099999999999996</v>
       </c>
       <c r="C13">
@@ -999,15 +995,15 @@
       <c r="M13">
         <v>12.76</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13">
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>13.07</v>
       </c>
       <c r="C14">
@@ -1043,15 +1039,15 @@
       <c r="M14">
         <v>8.9100000000000001</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14">
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>8.5199999999999996</v>
       </c>
       <c r="C15">
@@ -1084,15 +1080,15 @@
       <c r="M15">
         <v>16.27</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15">
         <v>9.5999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>6.1299999999999999</v>
       </c>
       <c r="C16">
@@ -1128,15 +1124,15 @@
       <c r="M16">
         <v>10.67</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16">
         <v>8.5700000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>14.98</v>
       </c>
       <c r="C17">
@@ -1172,15 +1168,15 @@
       <c r="M17">
         <v>10.51</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17">
         <v>9.5199999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>11.289999999999999</v>
       </c>
       <c r="C18">
@@ -1216,15 +1212,15 @@
       <c r="M18">
         <v>7.46</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18">
         <v>9.5500000000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>7.25</v>
       </c>
       <c r="C19">
@@ -1260,7 +1256,7 @@
       <c r="M19">
         <v>12.26</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19">
         <v>8.4000000000000004</v>
       </c>
     </row>
@@ -1290,8 +1286,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -1318,8 +1313,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>